<commit_message>
fix: data model from mappedBy to refBack
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CatalogueLocalHarmonizedVariables.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CatalogueLocalHarmonizedVariables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC74C0D-2E2C-6041-BBC9-4849D6805677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D234A26C-0B80-3D4E-967A-368F944A6E94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>InclusionCriteria</t>
   </si>
   <si>
-    <t>mappedBy</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>permittedValues</t>
+  </si>
+  <si>
+    <t>refBack</t>
   </si>
 </sst>
 </file>
@@ -853,7 +853,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,34 +873,34 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>18</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>2</v>
@@ -908,7 +908,7 @@
     </row>
     <row r="2" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>0</v>
@@ -923,12 +923,12 @@
         <v>1</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>6</v>
@@ -937,32 +937,32 @@
         <v>5</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>2</v>
@@ -971,43 +971,43 @@
         <v>7</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>0</v>
@@ -1022,51 +1022,51 @@
         <v>1</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
@@ -1085,21 +1085,21 @@
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1110,21 +1110,21 @@
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1135,21 +1135,21 @@
     </row>
     <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -1158,11 +1158,11 @@
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>11</v>
@@ -1174,12 +1174,12 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
@@ -1198,21 +1198,21 @@
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -1221,67 +1221,67 @@
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1295,19 +1295,19 @@
     </row>
     <row r="23" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -1316,33 +1316,33 @@
     </row>
     <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="8">
         <v>1</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J24" s="8" t="b">
         <v>1</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>5</v>
@@ -1354,12 +1354,12 @@
         <v>1</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>6</v>
@@ -1373,10 +1373,10 @@
     </row>
     <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>11</v>
@@ -1384,11 +1384,11 @@
     </row>
     <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>5</v>
@@ -1400,12 +1400,12 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>0</v>
@@ -1420,12 +1420,12 @@
         <v>1</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
@@ -1444,7 +1444,7 @@
     </row>
     <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
@@ -1463,11 +1463,11 @@
     </row>
     <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>9</v>
@@ -1482,10 +1482,10 @@
     </row>
     <row r="33" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>9</v>
@@ -1493,21 +1493,21 @@
     </row>
     <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
@@ -1516,21 +1516,21 @@
     </row>
     <row r="35" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -1539,34 +1539,34 @@
     </row>
     <row r="36" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>7</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
@@ -1606,7 +1606,7 @@
     </row>
     <row r="39" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8" t="s">
@@ -1625,7 +1625,7 @@
     </row>
     <row r="40" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
@@ -1644,16 +1644,16 @@
     </row>
     <row r="41" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>13</v>
@@ -1661,30 +1661,30 @@
     </row>
     <row r="42" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>7</v>
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>6</v>
@@ -1732,20 +1732,20 @@
         <v>2</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1771,7 +1771,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1780,27 +1780,27 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
         <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -1817,19 +1817,19 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -1874,7 +1874,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1883,141 +1883,141 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
       <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
-        <v>37</v>
-      </c>
       <c r="M1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
         <v>2</v>
       </c>
       <c r="Q1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
         <v>72</v>
-      </c>
-      <c r="C6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2044,30 +2044,30 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2092,16 +2092,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -2146,61 +2146,61 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="E1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2229,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>

</xml_diff>